<commit_message>
Finishing the full arch with the instruction register and its Rom_writer File
</commit_message>
<xml_diff>
--- a/additional_information/ALU_7bits.xlsx
+++ b/additional_information/ALU_7bits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6832E92-1C09-4484-80BD-EF7FEB0D3688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643FDF3F-A03F-4441-B104-336978468817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,7 +597,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finishing the new arch and wait for just adding the instruction
</commit_message>
<xml_diff>
--- a/additional_information/ALU_7bits.xlsx
+++ b/additional_information/ALU_7bits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643FDF3F-A03F-4441-B104-336978468817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C164011C-8007-4A76-9217-D8DF11CEF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Za</t>
   </si>
@@ -56,9 +56,6 @@
     <t>!A</t>
   </si>
   <si>
-    <t>!(X+Y)/(X&amp;Y)</t>
-  </si>
-  <si>
     <t>!OUT</t>
   </si>
   <si>
@@ -89,13 +86,10 @@
     <t>db++</t>
   </si>
   <si>
-    <t>Out_Low</t>
-  </si>
-  <si>
     <t>Catch_Flags</t>
   </si>
   <si>
-    <t>Out_High</t>
+    <t>!(A+DB)/(A&amp;DB)</t>
   </si>
 </sst>
 </file>
@@ -217,7 +211,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>119062</xdr:rowOff>
@@ -594,436 +588,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="40.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="46.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="40.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-      <c r="G10" s="5">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
-      <c r="J12" s="6" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
-        <v>1</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding some more touches to our arch, solve flags bug , optimize AL,AH with new control word and solve Instruction Register {on clock zero} problem
</commit_message>
<xml_diff>
--- a/additional_information/ALU_7bits.xlsx
+++ b/additional_information/ALU_7bits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C164011C-8007-4A76-9217-D8DF11CEF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC15B4A-E6D9-41FD-9CD8-061B09EAD3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,13 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
-  <si>
-    <t>Za</t>
-  </si>
-  <si>
-    <t>if set ALU output is connected to data bus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>if set X&amp;Y else X+Y</t>
   </si>
@@ -56,15 +50,9 @@
     <t>!A</t>
   </si>
   <si>
-    <t>!OUT</t>
-  </si>
-  <si>
     <t>!DB</t>
   </si>
   <si>
-    <t>Z_db</t>
-  </si>
-  <si>
     <t>A-DB</t>
   </si>
   <si>
@@ -86,10 +74,28 @@
     <t>db++</t>
   </si>
   <si>
-    <t>Catch_Flags</t>
-  </si>
-  <si>
-    <t>!(A+DB)/(A&amp;DB)</t>
+    <t>CPL_A</t>
+  </si>
+  <si>
+    <t>Z_D</t>
+  </si>
+  <si>
+    <t>CPL_D</t>
+  </si>
+  <si>
+    <t>AND_A_D</t>
+  </si>
+  <si>
+    <t>CPL_OUT</t>
+  </si>
+  <si>
+    <t>CATCH_FLAGS</t>
+  </si>
+  <si>
+    <t>Z_A</t>
+  </si>
+  <si>
+    <t>if set flags will be saved as long as</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,57 +614,57 @@
   <sheetData>
     <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -679,38 +685,38 @@
         <v>0</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -731,12 +737,12 @@
         <v>0</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -757,12 +763,12 @@
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -783,12 +789,12 @@
         <v>0</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -809,12 +815,12 @@
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -835,12 +841,12 @@
         <v>0</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -861,12 +867,12 @@
         <v>0</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
@@ -887,12 +893,12 @@
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5">
         <v>0</v>
@@ -913,12 +919,12 @@
         <v>1</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -939,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>